<commit_message>
Prem | Changes in create route
</commit_message>
<xml_diff>
--- a/micrograft/Cuttack/data.xlsx
+++ b/micrograft/Cuttack/data.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="300">
   <si>
     <t>Route Code</t>
   </si>
@@ -566,13 +566,390 @@
   </si>
   <si>
     <t>Via- Khuntakata-Athagarh-Kulailo-Khuntuni-Bali-Chowdwar-Manguli-Jagatpur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">କଟକ ସଦର- ଅର୍ଥଙ୍ଗ 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">କଟକ ସଦର-ଆୟତପୁର </t>
+  </si>
+  <si>
+    <t xml:space="preserve">କଟକ ସଦର- ଚାନ୍ଦୁଳି </t>
+  </si>
+  <si>
+    <t xml:space="preserve">କଟକ ସଦର-ବାମ୍ପକୁଦା </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ଆଠଗଡ-ଗୋବୋରା </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ଆଠଗଡ-ଅନନ୍ତପୁର </t>
+  </si>
+  <si>
+    <t>ଆଠଗଡ-ବଡ଼ଭୂଇଁଦେଶ  |</t>
+  </si>
+  <si>
+    <t>ବଡମ୍ବା -ଜୋଡୁମୁ |</t>
+  </si>
+  <si>
+    <t>ବଡମ୍ବା-ଚାନଚୁନିଆ |</t>
+  </si>
+  <si>
+    <t>ବଡମ୍ବା-ମାଲାଟି |</t>
+  </si>
+  <si>
+    <t>ବଡମ୍ବା-ବିଶ୍ୱନାଥପୁର |</t>
+  </si>
+  <si>
+    <t>ବାଙ୍କି-କଳାପଥର  |</t>
+  </si>
+  <si>
+    <t>ବାଙ୍କି-ପୁଇଞ୍ଚା |</t>
+  </si>
+  <si>
+    <t>ବାଙ୍କି-ବନସାପୁଟ |</t>
+  </si>
+  <si>
+    <t>ବାଙ୍କି-କାଣ୍ଟପାନହରା |</t>
+  </si>
+  <si>
+    <t>ବାରଙ୍ଗା-ସିସୋ |</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ବାରଙ୍ଗା-ନଛିପୁର </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>|</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">  ବାରଙ୍ଗା-ତାଲାଗର |</t>
+  </si>
+  <si>
+    <t>ଦାମପାରା-ପାଟପୁର  |</t>
+  </si>
+  <si>
+    <t>ଦାମପାରା-ତୁଳସୀପୁର  |</t>
+  </si>
+  <si>
+    <t>କଣ୍ଟାପଡା-ନହଲପୁର |</t>
+  </si>
+  <si>
+    <t>କଣ୍ଟାପଡା-ପୋଷ୍ଟାଲା |</t>
+  </si>
+  <si>
+    <t>କଣ୍ଟାପଡା-ଦିମିନି |</t>
+  </si>
+  <si>
+    <t>କୁଆଁପାଳ  - କୁରୁଜଙ୍ଗ |</t>
+  </si>
+  <si>
+    <t>କୁଆଁପାଳ  - ହଳଦିଆ  |</t>
+  </si>
+  <si>
+    <t>କୁଆଁପାଳ  - ଗୋଟାରା (ଅସୁଲପୁର)</t>
+  </si>
+  <si>
+    <t>ନରସିଂହପୁର-ଗୋଡିବନ୍ଧ</t>
+  </si>
+  <si>
+    <t>ନରସିଂହପୁର-ଦେବଭୂଇଁ  |</t>
+  </si>
+  <si>
+    <t>ନରସିଂହପୁର-ଚକାମୁଣ୍ଡା |</t>
+  </si>
+  <si>
+    <t>ନିଆଲି-ଏରଞ୍ଚା |</t>
+  </si>
+  <si>
+    <t>ନିଆଲି-ନିଭାରନ୍ |</t>
+  </si>
+  <si>
+    <t>ନିଆଲି-ତିହୁଡି |</t>
+  </si>
+  <si>
+    <t>ନିଆଲି-ନୂଆଗାଁ  |</t>
+  </si>
+  <si>
+    <t>ନିଶ୍ଚିନ୍ତକୋଇଲି  - ଉତରକୁଳ  |</t>
+  </si>
+  <si>
+    <t>ନିଶିଣ୍ଟାକୋଇଲି-କଟିକଟା |</t>
+  </si>
+  <si>
+    <t>ନିଶ୍ଚିନ୍ତକୋଇଲି-ତରାଟ |</t>
+  </si>
+  <si>
+    <t>ଚନ୍ଦ୍ରଦେଇପୁର  (ସାଲେପୁର) -ମହଜନପୁର |</t>
+  </si>
+  <si>
+    <t>ଚନ୍ଦ୍ରଦେଇପୁର  (ସାଲେପୁର) -ନାଇଗୁଆନ୍ |</t>
+  </si>
+  <si>
+    <t>ଚନ୍ଦ୍ରଦେଇପୁର  (ସାଲେପୁର) -ସୁଧାଖଣ୍ଡା |</t>
+  </si>
+  <si>
+    <t>ଟାଙ୍ଗୀ ଚୌଦ୍ୱାର -କାକାଡି |</t>
+  </si>
+  <si>
+    <t>ଟାଙ୍ଗୀ ଚୌଦ୍ୱାର -ବାଦାସାମନ୍ତପୁର |</t>
+  </si>
+  <si>
+    <t>ଟାଙ୍ଗୀ ଚୌଦ୍ୱାର - ଜରିପଦା  |</t>
+  </si>
+  <si>
+    <t>ଟାଙ୍ଗୀ ଚୌଦ୍ୱାର -କରଞ୍ଜୀ |</t>
+  </si>
+  <si>
+    <t>ପଞ୍ଚାଗାନ୍ (ଟିଗିରିଆ) -ସାମପୁର |</t>
+  </si>
+  <si>
+    <t>ପଞ୍ଚାଗାନ୍ (ଟିଗିରିଆ) -ହାଣ୍ଡପସି |</t>
+  </si>
+  <si>
+    <t>ପଞ୍ଚାଗାନ୍ (ଟିଗିରିଆ) -ଜମାଦେଇପୁର  |</t>
+  </si>
+  <si>
+    <t>ପଞ୍ଚାଗାନ୍ (ଟିଗିରିଆ) - ଗଦାଧରପୁର  |</t>
+  </si>
+  <si>
+    <t>ଆଠଗଡ -କଟକ |</t>
+  </si>
+  <si>
+    <t>ବଡମ୍ବା-କଟକ |</t>
+  </si>
+  <si>
+    <t>ବାଙ୍କୀ  -କଟକ |</t>
+  </si>
+  <si>
+    <t>ଦମପରା-କଟକ |</t>
+  </si>
+  <si>
+    <t>କଣ୍ଟାପଡା-କଟକ |</t>
+  </si>
+  <si>
+    <t>ମାହାଙ୍ଗା  -କଟକ |</t>
+  </si>
+  <si>
+    <t>ନରସିଂହପୁର-କଟକ |</t>
+  </si>
+  <si>
+    <t>ନିଆଳି  -କଟକ |</t>
+  </si>
+  <si>
+    <t>ନିଶ୍ଚିନ୍ତକୋଇଲି -କଟକ |</t>
+  </si>
+  <si>
+    <t>ସାଲେପୁର-କଟକ |</t>
+  </si>
+  <si>
+    <t>ଟାଙ୍ଗୀ ଚୌଦ୍ୱାର -କଟକ |</t>
+  </si>
+  <si>
+    <t>ଟିଗିରିଆ-କଟକ |</t>
+  </si>
+  <si>
+    <t>ଭାୟା - ବନାବିଧ୍ୟାଧରପୁର-ଗାତିରାଉଟପାଟନା-ମାତାଗାଜାପୁର-ପରମାନସା-ବିରିବତୀ-କନ୍ଦରପୁର-</t>
+  </si>
+  <si>
+    <t>ଭାୟା- ବନାବିଧ୍ୟାଧରପୁର-ଗାତିରାଉଟପାଟାନା-ବିରିବତୀ-ନିମାଇସାପୁର-କନ୍ଦରପୁର-</t>
+  </si>
+  <si>
+    <t>ଭାୟା- ନୁଆପଡା ଚାକା-ଘାଟାକୁଲା ଚାକା-ink ିଙ୍କିରିଆ ଚାକା-ଶ୍ରୀରାମ-ବେଣ୍ଟାକର ଚାକା-ସିସୁଆ-ତାଇଲାପଡା-ରାଉତାପୁର-ଡେଲୁଲି-ତାଇକାନା-କାଲାପଡା-ଧିଆ-ବାରାଲ-କୁଲାସୁରିଚୁଆନ୍-</t>
+  </si>
+  <si>
+    <t>ଭାୟା- ଗୋପାଳପୁର-ଶ୍ରୀକୋରୁଆନ୍-ଉରାଲୀ-ଜରିପଡା-ଖଣ୍ଡେଟା ଜିପି-ନାଗାବଲି-ସାଙ୍କତ୍ରାଶ-ନାଗାବଲି-ଆମାନା ଜିପି-ଅମାନପାରା-</t>
+  </si>
+  <si>
+    <t>ଭାୟା- ଡୋରାଡା-କୁଲାଇଲୋ-ଭୋଗ୍ରା ଏବଂ ପଛ ଡାଲାବାଗା-ଖୁଣ୍ଟୁନି-ରାଧାକିଶୋରପୁର-ଓରଣ୍ଡା-ଗୁରୁଦିଜାଟିଆ-ଛାଗୋନ୍-</t>
+  </si>
+  <si>
+    <t>ଭାୟା- ରାଧାଗୋବିନ୍ଦପୁର-ରାଜନାନଗର-ମହାକାଲାବାସ୍ତା-ଘଣ୍ଟିଖଲା-ଧୁରୁସିଆ-</t>
+  </si>
+  <si>
+    <t>ଭାୟା- ସାମସପୁର-ଇଚାପୁର-ଜେନାଡେଡେଶ-</t>
+  </si>
+  <si>
+    <t>ଭାୟା- ସାନାବରସିଂ-ରାଗଦୀପଡା-ଡିନାରୀ-ରାଗଦୀପଡା-ସାନାବରସିଂ-ବଡମ୍ବା-ସୁନାପାଲ-ଇଚାପୁର-ମଙ୍ଗରାଜପୁର-ସାଙ୍କାମୋରୀ-ଗୋପାମାଥୁରା-ଗୋପୀନାଥପୁର-ମୁଗାଗିରି-ବଙ୍ଗରିସିଂହା-ଯୋଡୁମୁ-ବଙ୍ଗରିସିଂହ-ମୁଗାଗାହିର-ଗୋପନାଥପୁର ଅଲ-ବଡମ୍ବା-</t>
+  </si>
+  <si>
+    <t>ଭାୟା- ସୁନାପାଲ-ଭଟ୍ଟାରିକା ଛକା-ବାଦକମ୍ବିଲୋ-ଟିନିଗରିଆ-ଟେଲିକମ୍ବିଲୋ-ମାଣ୍ଡିଆପାଲ୍ଲୀ-ଧେଣ୍ଡାଖମ୍ବା-</t>
+  </si>
+  <si>
+    <t>ଭାୟା- ସୁନାପାଲା ଛକା-କଦମ୍ପଲ-ଗୋପପୁର-କୃଷ୍ଣଚନ୍ଦ୍ରପୁର-ଦାମଙ୍ଗାଡିଆ-ରତାପତ-ଦଶରଥୀପୁର</t>
+  </si>
+  <si>
+    <t>ଭାୟା- ସୁନାପାଲା ଛକା-ଇଚାପୁର-ମଙ୍ଗରାଜପୁର-ଜାଜିଆ-କରାଡିବନ୍ଧା-ସାସଙ୍ଗା-ଭଟ୍ଟାରିକା-ଗେମି-କାନ୍ଦା-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ଭାୟା- ଅନୁରୀ-ଗୋଲାଗାଣ୍ଡା-ବ ide ଦେଶ୍ୱର-ବାଲାଭଦ୍ରପୁର-ଜଗନ୍ଥପୁର |_x000D_
+କେନ୍ଦୁ up ରୀ- </t>
+  </si>
+  <si>
+    <t>ଭାୟା- ବ୍ରହ୍ମପୁରା-କିଆପାଲା-ବାରପୁଟ-ନୁଆଗାନ୍-</t>
+  </si>
+  <si>
+    <t>ଭାୟା- ସୁବାମପୁର-ରତାଗର-ବୃନ୍ଦାବନ-</t>
+  </si>
+  <si>
+    <t>ଭାୟା- ଓଷ୍ଟିଆ-କାଦଲିବାଡି-</t>
+  </si>
+  <si>
+    <t>ଭାୟା- ଆରିଲୋ-ଗାବାବାସ୍ତା-ଦେଓକାଲୀ-କୋରାକାନା-ସିଙ୍ଗହୋଲ-ବାଇଲୋ ବଜାର-ଉଲାର-</t>
+  </si>
+  <si>
+    <t>ଭାୟା- ମହିଦାରବାରା-ନାଗରୀ-ଡାଲବାଦ୍-କୁରଙ୍ଗ-ପ୍ରଦାନ-ଗଙ୍ଗେଶ୍ୱର-</t>
+  </si>
+  <si>
+    <t>ଭାୟା- ପଞ୍ଚୁପାଲ-ବେଲଗାଖିଆ-ଗୋବିନ୍ଦପୁର ଏବଂ ରତନଗର-ମୁଣ୍ଡାଲି-</t>
+  </si>
+  <si>
+    <t>ଭାୟା- ଗୋବିନ୍ଦପୁର-ଦୁଲାନାପୁର-ତାଲାବସ୍ତା-ବିଲିପଡା-ହରିରାଜପୁର ଏବଂ ସିମିଲିପୁର-ଘସିପୁଟ-କୁସପାଙ୍ଗି-ଭାଗିପୁର-ବାମାରା-</t>
+  </si>
+  <si>
+    <t>ଭାୟା- ଘାସିପୁଟ-ନୁରସିଂହ-ଦୁର୍ଗାପୁର-ରାଗଡି-ଗୋପାଳପୁର-ଧନସାରା-</t>
+  </si>
+  <si>
+    <t>ଭାୟା- ବାଗଲପୁର-ବାଦପଟାସୁନ୍ଦର-har ାରପଡା-ଗୋବିନ୍ଦପୁର-ନୁଆଗାଙ୍ଗ୍ରାମ-</t>
+  </si>
+  <si>
+    <t>ଭାୟା- ବ୍ରାହ୍ମଣସାଲୋ-ବ୍ରାହ୍ମଣବତୀ-</t>
+  </si>
+  <si>
+    <t>ଭାୟା- ଉର୍ଧା-ଆଦାସପୁର-ଉତ୍ତରାଣା-</t>
+  </si>
+  <si>
+    <t>ଭାୟା- ଚାହାପଡା (ଛତ୍ରୋଟା) -ମହଙ୍ଗା-ବାରାହିପୁର-ଓସଙ୍ଗା-ଗୋକାନ୍ (ଇରାକାନା) -ପୋଡାମରାଇ-ନାହଙ୍ଗା (ଗୋଦାଗୋପା ବଜାର) -ଭଦ୍ରାଶ୍ୱର-ଗୋପାଳପୁର-</t>
+  </si>
+  <si>
+    <t>ଭାୟା- କୁସୁପୁର-ବାଲିଚନ୍ଦ୍ରପୁର-ପାନସପୁର-ଲଲିତଗିରି-ଓଲାକାନା-</t>
+  </si>
+  <si>
+    <t>ଭାୟା- ଚାହାପଡା (ଛତ୍ରୋଟା) -ମାଙ୍ଗା-ଓସଙ୍ଗା-ପଲ୍ଲିସାହି-ଭ un ନରିଆ-ଉମାରା-ଗୋଟାରା (ଅସୁଲପୁର) -</t>
+  </si>
+  <si>
+    <t>ଭାୟା- ପାଇକାପଡାପାଟାନା-ଆଲାରା-ବାନ୍ଧହୁଦା-ଆଡେଇସୁଣ୍ଡି ସାଗର-ବୋକଡା-</t>
+  </si>
+  <si>
+    <t>ଭାୟା- ପାକାପଡା ପାଟନା, ନିଜିଗର-ବାଦାବୁଇନ୍, ରଣସିଗପୁର-ଜାଜିବନ୍ଧା-ବିରସିଂହପୁର-ଭୁସ୍କା-</t>
+  </si>
+  <si>
+    <t>ଭାୟା- ନୁଆପାଟନା-ନିମାସାହି-କୋକଲବା-କଥଖୁଣ୍ଟା-ବାଲିସାହି-ସାରଦାପୁର-ଯୋଡମ୍-</t>
+  </si>
+  <si>
+    <t>ଭାୟା- ବିଲାସୁନି-ରାନିଓଲା-କାସରଡା-</t>
+  </si>
+  <si>
+    <t>ଭାୟା- ଜଲାରପୁର-ମାଧବା-ରତନପୁର-କେ ପ୍ରସାଦ-ବିନିଶପୁର-</t>
+  </si>
+  <si>
+    <t>ଭାୟା- ଜଲାରପୁର-କାପାସୀ-ସାଧନା-</t>
+  </si>
+  <si>
+    <t>ଭାୟା - ବାହରାନା- ପୋଖରିଗାଓଁ-ପହଙ୍ଗା-ଏକବେରୁଆନ୍-ସୀଥାଲୋ-ସାଗାଦାଇଲୋ-ବିଲାସୁନି-ଆଲାନା-ଆନ୍ଲୋ-</t>
+  </si>
+  <si>
+    <t>ଭାୟା- ନେମାଲ-ସାନ୍ତାପୁର-ପାଲଡା-ବାବୁଜାଙ୍ଗ-ମଣିଜଙ୍ଗା-</t>
+  </si>
+  <si>
+    <t>ଭାୟା- ବୁହାଲୋ-ତିଲକାନା-ବାନ୍ଧକାଟିଆ-ତରାଟ-ଅସୁରଶ୍ୱର-</t>
+  </si>
+  <si>
+    <t>ଭାୟା- ବୁହାଲୋ-ନେମାଲୋ-ନାଗାସପୁର-ଦ ud ଦପୁର-ନରେନ୍ଦ୍ରପୁର-ଅର୍ଟି-କେନୋ-</t>
+  </si>
+  <si>
+    <t>ଭାୟା- ବାଲିସାହି-ସିସୁଆ-ସ uri ରୀ ଏବଂ ନନ୍ଦୋଲ-ମହାନ୍-କତାରପା-ଓଡିସିଂହ-ମାଲାସାନ-ନରଡା-ରମେଶ୍ୱର-ଗୋପୀନାଥପୁର-ସତ୍ୟଭାମପୁର-ବାହୁଗ୍ରାମ-</t>
+  </si>
+  <si>
+    <t>ଭାୟା- ବୋଡାମୁଣ୍ଡେଇ- ପାଇକଲ୍-ରାଇସୁଙ୍ଗୁରା-ମିର୍ଜାପୁର-ଭୀମଦାସପୁର-ସିଦ୍ଧୋ-ଖାନିପୁର-</t>
+  </si>
+  <si>
+    <t>ଭାୟା- ବାଲିସାହି-ସିସୁଆ-ଟାରିଟୋ-ରତିଲୋ-ପୁରୂନାହାଟ-</t>
+  </si>
+  <si>
+    <t>ଭାୟା- କୋଟାସାହି-କାନହିପୁର-ସାଲାଗାଓଁ-ନାଖ୍ରା-ଆଗ୍ରାହତ-ଇନ୍ଦ୍ରାନିପାଟନ-କାୟଲପଡା-ଧବାଲେଶ୍ୱର-</t>
+  </si>
+  <si>
+    <t>ଭାୟା- କୋଟାସାହି-କାନହିପୁର- ଗରୁଡାଗାଓନ୍-ବରହମପୁର-ମହିସାଲାଣ୍ଡା-ଶଙ୍କରପୁର-ମଙ୍ଗରାଜପୁର-</t>
+  </si>
+  <si>
+    <t>ଭାୟା- କୋଟାସାହି-ଉଚାପଡା-ମାଗୁରା-</t>
+  </si>
+  <si>
+    <t>ଭାୟା- କୋଟାସାହି-କାନହିପୁର-ଗାରୁଦାଗୋନ୍-ସଫା-</t>
+  </si>
+  <si>
+    <t>ଭାୟା- ମହଲଦୀପା-ସମପଡା-ଖାନ୍ଦାହାଟା-ବାଦାନାପୁଟ-</t>
+  </si>
+  <si>
+    <t>ଭାୟା- ନୁଆସାଦକ୍-ଗୋଡିଜରିଆ-ଭିରୁଦା-ଆଚାଲକୋଟ୍-</t>
+  </si>
+  <si>
+    <t>ଭାୟା- ପାସ୍-ବାଲିପୁଟ-ପଙ୍କଲ-ଭେଜିଆ-ଭୋଗଡା-ନୁଆପାଟାନା ଦ୍ୱାରା ନିଜିଗଡ଼-ବିନ୍ଦାନିମା-</t>
+  </si>
+  <si>
+    <t>ଭାୟା- ନିଜିଗଡ଼-ପୁରାଣତିଗିରିଆ-ପାଇକାନାରା-ବାଦାନୁଆପୁଟ-ସନ୍ଥିପାଲା-</t>
+  </si>
+  <si>
+    <t>ଭାୟା- କାଣ୍ଟୋଲ-କାଖଡି-ମହାକାଲାବାସ୍ତା |</t>
+  </si>
+  <si>
+    <t>ଭାୟା- ଧୋବନିନାଲା-ମାନୀଆବନ୍ଧ-ବିଧରପୁର-ନୂଆପାଟଣା -ବିରିପୁଟ-ନୂଆସଡ଼କ 
+ -ଖୁଣ୍ଟାକାଟା-ଆଠଗଡ-କାଣ୍ଟୋଲ-କାରିକୋଲ-ମହାକାଲାବାସ୍ତା-ନିଧିପୁର -କାଖଡି</t>
+  </si>
+  <si>
+    <t>ଭାୟା- ଜଟାମୁଣ୍ଡିଆ-ପଥପୁର -ଦେବିଦ୍ୱାର-ବଅଁରା- ଗୋବିନ୍ଦପୁର-ଗୋଡିସାହି-ସନ୍ଧପୁର-ତ୍ରିସୁଳିଆ |</t>
+  </si>
+  <si>
+    <t>ଭାୟା - ପୁସପାଙ୍ଗି-ଗୋଡିସାହି-ସାନ୍ଧପୁର-ତ୍ରିସୁଲିଆ |</t>
+  </si>
+  <si>
+    <t>ଭାୟା- ସୁନ୍ଦରଗାଓଁ-ବ୍ରାହ୍ମଣଜ୍ରିଲୋ-ଫୁଲନଖରା- ଗୋପାଳପୁର |</t>
+  </si>
+  <si>
+    <t>ଭାୟା- ଧର୍ମଘଟପୁର-ମନୋହରପୁର-ସାଲେପୁର -ସିସୁଆ-ଭାଟପଡା -ଖରଡିଆ  - ଭଇରପୁର -ଜଗତପୁର</t>
+  </si>
+  <si>
+    <t>ଭାୟା-ରୁଖପଡା-ବାଗଧାରିଆ-ଚମ୍ପେଶ୍ୱର-ବାଲିଜାରୀ-ବଡମ୍ବା-ମଣିବନ୍ଧା-ନୁଆପାଟନା-ତିଗିରା- ଖୁଣ୍ଟକଟା -ଆଠଗଡ-କୁଲେଇଲ -ଖୁଣ୍ଟୁଣି-ବାଲି- ଚୌଦ୍ୱାର-ମଙ୍ଗୁଲି-ଜଗତପୁର</t>
+  </si>
+  <si>
+    <t>ଭାୟା- ଅଡସପୁର -ଓଲଟପୁର-କଣ୍ଟାପଡା-ସୁନ୍ଦରଗାଁ - ବ୍ରାହ୍ମଣଝରିଲୋ -ଫୁଲନଖରା-ଗୋପାଳପୁର</t>
+  </si>
+  <si>
+    <t>ଭାୟା- କେନ୍ଦୁପଟାନା -ସାଲେପୁର-ସିସୁଆ-ଭଟ୍ଟପଡା-ଖରାହିଆ ଭଇରପୁର -ଜଗତପୁର</t>
+  </si>
+  <si>
+    <t>ଭାୟା- ସିସୁଆ-ଭଟ୍ଟପଡା-ଖରାହିଆ-ଭଇରପୁର -ଜଗତପୁର |</t>
+  </si>
+  <si>
+    <t>ଭାୟା - କପିଲାଶ ରୋଡ-ସୋସିଆପଡା-ହରିପୁର-ସଫା-ବିସି ନାହକାନି-ହଳଦିବସନ୍ତ -କାମୋମଗୋ-ଡାଲିଜୋଡା-ବରହମପୁର-ଚାରବାଟିଆ-ଆଗ୍ରାହାଟ - ଏ ର ସି ଚୌଦ୍ୱାର- ମଙ୍ଗୁଳି -ଜଗତପୁର |</t>
+  </si>
+  <si>
+    <t>ଭାୟା- ଖୁଣ୍ଟାକାଟା-ଅଟାଗର-କୁଲାଇଲୋ-ଖୁଣ୍ଟୁନି-ବାଲି-ଚୌଦ୍ୱାର-ମାଙ୍ଗୁଲି-ଜଗତପୁର |</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -580,16 +957,40 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -597,13 +998,55 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -876,7 +1319,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -886,8 +1329,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C67" sqref="C67"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -896,7 +1339,7 @@
     <col min="2" max="2" width="37.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="84.85546875" customWidth="1"/>
     <col min="4" max="4" width="33.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="64.140625" customWidth="1"/>
+    <col min="5" max="5" width="66" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -916,7 +1359,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -926,8 +1369,14 @@
       <c r="C2" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D2" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -937,8 +1386,14 @@
       <c r="C3" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D3" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -948,8 +1403,14 @@
       <c r="C4" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D4" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -959,8 +1420,14 @@
       <c r="C5" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D5" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -969,6 +1436,12 @@
       </c>
       <c r="C6" t="s">
         <v>127</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -981,6 +1454,12 @@
       <c r="C7" t="s">
         <v>128</v>
       </c>
+      <c r="D7" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -992,8 +1471,14 @@
       <c r="C8" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D8" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -1003,8 +1488,14 @@
       <c r="C9" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D9" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -1014,8 +1505,14 @@
       <c r="C10" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D10" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -1025,8 +1522,14 @@
       <c r="C11" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D11" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -1036,8 +1539,14 @@
       <c r="C12" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D12" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="45.75" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -1046,6 +1555,12 @@
       </c>
       <c r="C13" t="s">
         <v>134</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1058,6 +1573,12 @@
       <c r="C14" t="s">
         <v>135</v>
       </c>
+      <c r="D14" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>253</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -1069,6 +1590,12 @@
       <c r="C15" t="s">
         <v>136</v>
       </c>
+      <c r="D15" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>254</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -1080,8 +1607,14 @@
       <c r="C16" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -1091,8 +1624,14 @@
       <c r="C17" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -1102,8 +1641,14 @@
       <c r="C18" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -1113,8 +1658,14 @@
       <c r="C19" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -1124,8 +1675,14 @@
       <c r="C20" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -1135,8 +1692,14 @@
       <c r="C21" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -1146,8 +1709,14 @@
       <c r="C22" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>26</v>
       </c>
@@ -1157,8 +1726,14 @@
       <c r="C23" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>27</v>
       </c>
@@ -1168,8 +1743,14 @@
       <c r="C24" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>28</v>
       </c>
@@ -1179,8 +1760,14 @@
       <c r="C25" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D25" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>29</v>
       </c>
@@ -1190,8 +1777,14 @@
       <c r="C26" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D26" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>30</v>
       </c>
@@ -1201,8 +1794,14 @@
       <c r="C27" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D27" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>31</v>
       </c>
@@ -1212,8 +1811,14 @@
       <c r="C28" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D28" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>32</v>
       </c>
@@ -1223,8 +1828,14 @@
       <c r="C29" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D29" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>33</v>
       </c>
@@ -1234,8 +1845,14 @@
       <c r="C30" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D30" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>34</v>
       </c>
@@ -1245,8 +1862,14 @@
       <c r="C31" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D31" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>35</v>
       </c>
@@ -1256,8 +1879,14 @@
       <c r="C32" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D32" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>36</v>
       </c>
@@ -1267,8 +1896,14 @@
       <c r="C33" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D33" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>37</v>
       </c>
@@ -1278,8 +1913,14 @@
       <c r="C34" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D34" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>38</v>
       </c>
@@ -1289,8 +1930,14 @@
       <c r="C35" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D35" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="E35" s="7" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>39</v>
       </c>
@@ -1300,8 +1947,14 @@
       <c r="C36" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D36" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="E36" s="7" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>40</v>
       </c>
@@ -1311,8 +1964,14 @@
       <c r="C37" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D37" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="E37" s="7" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>41</v>
       </c>
@@ -1322,8 +1981,14 @@
       <c r="C38" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D38" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="E38" s="10" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>42</v>
       </c>
@@ -1333,8 +1998,14 @@
       <c r="C39" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D39" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="E39" s="7" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>43</v>
       </c>
@@ -1344,8 +2015,14 @@
       <c r="C40" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D40" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E40" s="8" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>44</v>
       </c>
@@ -1355,8 +2032,14 @@
       <c r="C41" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D41" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>45</v>
       </c>
@@ -1366,8 +2049,14 @@
       <c r="C42" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D42" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="E42" s="7" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>46</v>
       </c>
@@ -1377,8 +2066,14 @@
       <c r="C43" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D43" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="E43" s="7" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>47</v>
       </c>
@@ -1388,8 +2083,14 @@
       <c r="C44" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D44" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="E44" s="7" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>48</v>
       </c>
@@ -1399,8 +2100,14 @@
       <c r="C45" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D45" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="E45" s="7" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>49</v>
       </c>
@@ -1410,8 +2117,14 @@
       <c r="C46" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D46" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="E46" s="7" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>50</v>
       </c>
@@ -1421,8 +2134,14 @@
       <c r="C47" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D47" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="E47" s="7" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>51</v>
       </c>
@@ -1432,8 +2151,14 @@
       <c r="C48" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D48" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="E48" s="7" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>52</v>
       </c>
@@ -1443,8 +2168,14 @@
       <c r="C49" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D49" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="E49" s="7" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>53</v>
       </c>
@@ -1454,8 +2185,14 @@
       <c r="C50" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D50" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="E50" s="7" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>54</v>
       </c>
@@ -1465,8 +2202,14 @@
       <c r="C51" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D51" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="E51" s="7" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>55</v>
       </c>
@@ -1476,8 +2219,14 @@
       <c r="C52" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D52" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="E52" s="7" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>56</v>
       </c>
@@ -1487,8 +2236,14 @@
       <c r="C53" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D53" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="E53" s="7" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>57</v>
       </c>
@@ -1498,8 +2253,14 @@
       <c r="C54" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D54" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="E54" s="7" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>58</v>
       </c>
@@ -1509,8 +2270,14 @@
       <c r="C55" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D55" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="E55" s="7" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>59</v>
       </c>
@@ -1520,8 +2287,14 @@
       <c r="C56" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D56" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="E56" s="7" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>60</v>
       </c>
@@ -1531,8 +2304,14 @@
       <c r="C57" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D57" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="E57" s="7" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>61</v>
       </c>
@@ -1542,8 +2321,14 @@
       <c r="C58" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D58" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="E58" s="7" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>62</v>
       </c>
@@ -1553,8 +2338,14 @@
       <c r="C59" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D59" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="E59" s="7" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>63</v>
       </c>
@@ -1563,6 +2354,12 @@
       </c>
       <c r="C60" t="s">
         <v>181</v>
+      </c>
+      <c r="D60" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>299</v>
       </c>
     </row>
   </sheetData>

</xml_diff>